<commit_message>
Remove index.tx and remove absolute references to value sets
Remove index.tx and remove absolute references to value sets e35a3362c511aef45fd11d900e5fcf4ae740639b
</commit_message>
<xml_diff>
--- a/ig/feature/sos-medecins/StructureDefinition-sas-sos-appointment.xlsx
+++ b/ig/feature/sos-medecins/StructureDefinition-sas-sos-appointment.xlsx
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-11-08T09:39:39+00:00</t>
+    <t>2023-11-08T15:44:44+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -731,7 +731,7 @@
     <t>Allows for alternative encodings within a code system, and translations to other code systems.</t>
   </si>
   <si>
-    <t>http://interop.esante.gouv.fr/ig/fhir/sas/ValueSet/sas-sos-valueset-typeidentifiant</t>
+    <t>https://interop.esante.gouv.fr/ig/fhir/sas/ValueSet/sas-sos-valueset-typeidentifiant</t>
   </si>
   <si>
     <t>CodeableConcept.coding</t>
@@ -1406,7 +1406,7 @@
     <t>Participation status of the actor.</t>
   </si>
   <si>
-    <t>http://interop.esante.gouv.fr/ig/fhir/sas/ValueSet/sas-sos-valueset-participant-status</t>
+    <t>https://interop.esante.gouv.fr/ig/fhir/sas/ValueSet/sas-sos-valueset-participant-status</t>
   </si>
   <si>
     <t>Appointment.participant.period</t>
@@ -1763,7 +1763,7 @@
     <col min="23" max="23" width="19.03515625" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="18.859375" customWidth="true" bestFit="true"/>
     <col min="25" max="25" width="98.375" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="78.2734375" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="79.23046875" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="6.34765625" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="22.71875" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="42.03515625" customWidth="true" bestFit="true"/>

</xml_diff>